<commit_message>
modification tableau de répartitions
</commit_message>
<xml_diff>
--- a/Rendu FINAL/Développement/repart.xlsx
+++ b/Rendu FINAL/Développement/repart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="60">
   <si>
     <t>Rendu Finale: Développement + Tests</t>
   </si>
@@ -84,18 +84,6 @@
     <t>Rapport Conception BD</t>
   </si>
   <si>
-    <t>Développement BL</t>
-  </si>
-  <si>
-    <t>Développement</t>
-  </si>
-  <si>
-    <t>Développement Persistance</t>
-  </si>
-  <si>
-    <t>Développement GUI</t>
-  </si>
-  <si>
     <t>Rapport Analyse</t>
   </si>
   <si>
@@ -199,13 +187,22 @@
   </si>
   <si>
     <t>Mettre en place gestionnaire de version</t>
+  </si>
+  <si>
+    <t>Développement demande de réservation</t>
+  </si>
+  <si>
+    <t>Développement Menu + Login</t>
+  </si>
+  <si>
+    <t>Développement consulter planning</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,16 +210,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -230,13 +259,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,23 +643,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D61"/>
+  <dimension ref="B1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="90.85546875" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
@@ -570,7 +677,7 @@
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -578,7 +685,7 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -586,7 +693,7 @@
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -594,7 +701,7 @@
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -602,7 +709,7 @@
       <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -610,7 +717,7 @@
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -618,7 +725,7 @@
       <c r="C10" t="s">
         <v>13</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -626,7 +733,7 @@
       <c r="C11" t="s">
         <v>14</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -634,7 +741,7 @@
       <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -642,7 +749,7 @@
       <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -650,7 +757,7 @@
       <c r="C14" t="s">
         <v>17</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -658,7 +765,7 @@
       <c r="C15" t="s">
         <v>18</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -666,7 +773,7 @@
       <c r="C16" t="s">
         <v>19</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -674,335 +781,355 @@
       <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>21</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+      <c r="C19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="9"/>
+      <c r="D20" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="9"/>
+      <c r="D21" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="12"/>
+      <c r="D22" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="12"/>
+      <c r="D24" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="12"/>
+      <c r="D26" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="D19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" t="s">
-        <v>4</v>
+        <v>23</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" t="s">
-        <v>12</v>
+        <v>24</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" t="s">
-        <v>12</v>
+        <v>25</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" t="s">
-        <v>12</v>
+        <v>27</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" t="s">
-        <v>4</v>
+        <v>28</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" t="s">
-        <v>10</v>
+        <v>29</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" t="s">
-        <v>4</v>
+        <v>30</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" t="s">
-        <v>6</v>
+        <v>31</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>40</v>
-      </c>
-      <c r="D38" t="s">
-        <v>6</v>
+        <v>32</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>41</v>
-      </c>
-      <c r="D40" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>42</v>
-      </c>
-      <c r="D41" t="s">
-        <v>10</v>
+        <v>35</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>43</v>
-      </c>
-      <c r="D42" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>44</v>
-      </c>
-      <c r="D43" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>45</v>
-      </c>
-      <c r="D44" t="s">
-        <v>6</v>
+      <c r="C44" s="6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>46</v>
-      </c>
-      <c r="D45" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>47</v>
-      </c>
-      <c r="D46" t="s">
+        <v>39</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>48</v>
-      </c>
-      <c r="D47" t="s">
-        <v>4</v>
+        <v>40</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
+        <v>41</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>43</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>44</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>45</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>46</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>47</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>28</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>39</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>48</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
         <v>49</v>
       </c>
-      <c r="D48" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
+      <c r="D58" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
         <v>50</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D59" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
         <v>51</v>
       </c>
-      <c r="D50" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
-        <v>32</v>
-      </c>
-      <c r="D51" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
-        <v>43</v>
-      </c>
-      <c r="D52" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
+      <c r="D60" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
         <v>52</v>
       </c>
-      <c r="D53" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
+      <c r="D61" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
         <v>53</v>
       </c>
-      <c r="D54" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
+      <c r="D62" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
         <v>54</v>
       </c>
-      <c r="D55" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
+      <c r="D63" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
         <v>55</v>
       </c>
-      <c r="D56" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
+      <c r="C65" t="s">
         <v>56</v>
       </c>
-      <c r="D57" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
-        <v>57</v>
-      </c>
-      <c r="D58" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>60</v>
+      <c r="D65" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>